<commit_message>
Updated files and tables
</commit_message>
<xml_diff>
--- a/data/Supplemental File 2_Differentially Expressed Ciliome 1.19.22.manuallycurated.xlsx
+++ b/data/Supplemental File 2_Differentially Expressed Ciliome 1.19.22.manuallycurated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelseytroyer/Dropbox/Dev Cell-Resource-CiliaHet-2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Konrad\Shiny_Sam\Ciliome_Gene_Expression\data_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FBDD97A-14AE-154B-9D6B-F9F49C27E594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{013FA114-1AB1-445E-83D7-C47A66E2BE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="640" windowWidth="16780" windowHeight="14800" xr2:uid="{1EE52754-5ACE-2745-9AA3-C3D33E295F23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1EE52754-5ACE-2745-9AA3-C3D33E295F23}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW_DE CILIOME" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="612">
   <si>
     <t>PKHD1</t>
   </si>
@@ -1914,6 +1914,9 @@
   <si>
     <t>DNAI3</t>
   </si>
+  <si>
+    <t>colors</t>
+  </si>
 </sst>
 </file>
 
@@ -1922,7 +1925,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1967,6 +1970,14 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2000,7 +2011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2029,6 +2040,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2347,54 +2361,54 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="M178" sqref="M178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
     <col min="2" max="2" width="20" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="1"/>
+    <col min="10" max="10" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="45.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>143</v>
       </c>
@@ -2422,8 +2436,11 @@
       <c r="I8" s="4" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="20" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>443</v>
       </c>
@@ -2449,9 +2466,11 @@
         <v>289</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>444</v>
       </c>
@@ -2477,9 +2496,11 @@
         <v>289</v>
       </c>
       <c r="I10" s="7"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>445</v>
       </c>
@@ -2505,9 +2526,11 @@
         <v>289</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>446</v>
       </c>
@@ -2533,9 +2556,11 @@
         <v>289</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>447</v>
       </c>
@@ -2561,9 +2586,11 @@
         <v>289</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>448</v>
       </c>
@@ -2589,9 +2616,11 @@
         <v>151</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>150</v>
       </c>
@@ -2615,9 +2644,11 @@
         <v>289</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>449</v>
       </c>
@@ -2643,9 +2674,11 @@
         <v>289</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>450</v>
       </c>
@@ -2671,9 +2704,11 @@
         <v>289</v>
       </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>451</v>
       </c>
@@ -2699,9 +2734,11 @@
         <v>289</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>452</v>
       </c>
@@ -2727,9 +2764,11 @@
         <v>289</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>152</v>
       </c>
@@ -2753,9 +2792,11 @@
         <v>289</v>
       </c>
       <c r="I20" s="7"/>
-      <c r="J20" s="16"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>453</v>
       </c>
@@ -2781,9 +2822,11 @@
         <v>289</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>153</v>
       </c>
@@ -2805,9 +2848,11 @@
         <v>289</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>154</v>
       </c>
@@ -2829,9 +2874,11 @@
         <v>289</v>
       </c>
       <c r="I23" s="7"/>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>155</v>
       </c>
@@ -2855,9 +2902,11 @@
         <v>289</v>
       </c>
       <c r="I24" s="7"/>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>454</v>
       </c>
@@ -2883,9 +2932,11 @@
         <v>289</v>
       </c>
       <c r="I25" s="11"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>156</v>
       </c>
@@ -2907,9 +2958,11 @@
         <v>289</v>
       </c>
       <c r="I26" s="11"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>455</v>
       </c>
@@ -2935,9 +2988,11 @@
         <v>289</v>
       </c>
       <c r="I27" s="7"/>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>456</v>
       </c>
@@ -2963,9 +3018,11 @@
         <v>151</v>
       </c>
       <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>457</v>
       </c>
@@ -2991,9 +3048,11 @@
         <v>289</v>
       </c>
       <c r="I29" s="11"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>458</v>
       </c>
@@ -3019,9 +3078,11 @@
         <v>289</v>
       </c>
       <c r="I30" s="11"/>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>157</v>
       </c>
@@ -3047,9 +3108,11 @@
       <c r="I31" s="11" t="s">
         <v>604</v>
       </c>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>158</v>
       </c>
@@ -3071,9 +3134,11 @@
         <v>289</v>
       </c>
       <c r="I32" s="11"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>459</v>
       </c>
@@ -3099,9 +3164,11 @@
         <v>289</v>
       </c>
       <c r="I33" s="7"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>460</v>
       </c>
@@ -3127,9 +3194,11 @@
         <v>151</v>
       </c>
       <c r="I34" s="11"/>
-      <c r="J34" s="16"/>
-    </row>
-    <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>262</v>
       </c>
@@ -3151,9 +3220,11 @@
         <v>289</v>
       </c>
       <c r="I35" s="13"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>461</v>
       </c>
@@ -3179,9 +3250,11 @@
         <v>289</v>
       </c>
       <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>462</v>
       </c>
@@ -3207,9 +3280,11 @@
         <v>151</v>
       </c>
       <c r="I37" s="13"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>264</v>
       </c>
@@ -3231,9 +3306,11 @@
         <v>289</v>
       </c>
       <c r="I38" s="11"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>463</v>
       </c>
@@ -3259,9 +3336,11 @@
         <v>289</v>
       </c>
       <c r="I39" s="7"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>464</v>
       </c>
@@ -3287,9 +3366,11 @@
         <v>289</v>
       </c>
       <c r="I40" s="13"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>159</v>
       </c>
@@ -3311,9 +3392,11 @@
         <v>289</v>
       </c>
       <c r="I41" s="7"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>465</v>
       </c>
@@ -3339,9 +3422,11 @@
         <v>289</v>
       </c>
       <c r="I42" s="13"/>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>466</v>
       </c>
@@ -3367,9 +3452,11 @@
         <v>289</v>
       </c>
       <c r="I43" s="13"/>
-      <c r="J43" s="16"/>
-    </row>
-    <row r="44" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>239</v>
       </c>
@@ -3393,9 +3480,11 @@
         <v>289</v>
       </c>
       <c r="I44" s="11"/>
-      <c r="J44" s="8"/>
-    </row>
-    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>160</v>
       </c>
@@ -3419,9 +3508,11 @@
       <c r="I45" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>161</v>
       </c>
@@ -3443,9 +3534,11 @@
         <v>289</v>
       </c>
       <c r="I46" s="7"/>
-      <c r="J46" s="16"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>284</v>
       </c>
@@ -3467,9 +3560,11 @@
         <v>289</v>
       </c>
       <c r="I47" s="11"/>
-      <c r="J47" s="16"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>162</v>
       </c>
@@ -3495,9 +3590,11 @@
       <c r="I48" s="14" t="s">
         <v>605</v>
       </c>
-      <c r="J48" s="16"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>467</v>
       </c>
@@ -3523,9 +3620,11 @@
         <v>289</v>
       </c>
       <c r="I49" s="11"/>
-      <c r="J49" s="16"/>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>468</v>
       </c>
@@ -3551,9 +3650,11 @@
         <v>289</v>
       </c>
       <c r="I50" s="13"/>
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>469</v>
       </c>
@@ -3581,9 +3682,11 @@
       <c r="I51" s="13" t="s">
         <v>606</v>
       </c>
-      <c r="J51" s="16"/>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>470</v>
       </c>
@@ -3609,9 +3712,11 @@
         <v>289</v>
       </c>
       <c r="I52" s="13"/>
-      <c r="J52" s="8"/>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>163</v>
       </c>
@@ -3637,9 +3742,11 @@
       <c r="I53" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J53" s="8"/>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>164</v>
       </c>
@@ -3663,9 +3770,11 @@
         <v>289</v>
       </c>
       <c r="I54" s="7"/>
-      <c r="J54" s="8"/>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>165</v>
       </c>
@@ -3689,9 +3798,11 @@
         <v>289</v>
       </c>
       <c r="I55" s="13"/>
-      <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>166</v>
       </c>
@@ -3713,9 +3824,11 @@
         <v>289</v>
       </c>
       <c r="I56" s="13"/>
-      <c r="J56" s="16"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>471</v>
       </c>
@@ -3741,9 +3854,11 @@
         <v>289</v>
       </c>
       <c r="I57" s="13"/>
-      <c r="J57" s="16"/>
-    </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>472</v>
       </c>
@@ -3769,9 +3884,11 @@
         <v>289</v>
       </c>
       <c r="I58" s="7"/>
-      <c r="J58" s="8"/>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>265</v>
       </c>
@@ -3793,9 +3910,11 @@
         <v>289</v>
       </c>
       <c r="I59" s="13"/>
-      <c r="J59" s="8"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>473</v>
       </c>
@@ -3821,9 +3940,11 @@
         <v>289</v>
       </c>
       <c r="I60" s="13"/>
-      <c r="J60" s="16"/>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>167</v>
       </c>
@@ -3845,9 +3966,11 @@
         <v>289</v>
       </c>
       <c r="I61" s="13"/>
-      <c r="J61" s="8"/>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>283</v>
       </c>
@@ -3869,9 +3992,11 @@
         <v>289</v>
       </c>
       <c r="I62" s="13"/>
-      <c r="J62" s="8"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>474</v>
       </c>
@@ -3897,9 +4022,11 @@
         <v>289</v>
       </c>
       <c r="I63" s="13"/>
-      <c r="J63" s="16"/>
-    </row>
-    <row r="64" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>475</v>
       </c>
@@ -3925,9 +4052,11 @@
         <v>289</v>
       </c>
       <c r="I64" s="11"/>
-      <c r="J64" s="8"/>
-    </row>
-    <row r="65" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>476</v>
       </c>
@@ -3953,9 +4082,11 @@
         <v>289</v>
       </c>
       <c r="I65" s="7"/>
-      <c r="J65" s="8"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>477</v>
       </c>
@@ -3981,9 +4112,11 @@
         <v>289</v>
       </c>
       <c r="I66" s="11"/>
-      <c r="J66" s="16"/>
-    </row>
-    <row r="67" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>478</v>
       </c>
@@ -4009,9 +4142,11 @@
         <v>289</v>
       </c>
       <c r="I67" s="7"/>
-      <c r="J67" s="8"/>
-    </row>
-    <row r="68" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>260</v>
       </c>
@@ -4037,9 +4172,11 @@
         <v>289</v>
       </c>
       <c r="I68" s="11"/>
-      <c r="J68" s="8"/>
-    </row>
-    <row r="69" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>479</v>
       </c>
@@ -4065,9 +4202,11 @@
         <v>289</v>
       </c>
       <c r="I69" s="7"/>
-      <c r="J69" s="8"/>
-    </row>
-    <row r="70" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>480</v>
       </c>
@@ -4093,9 +4232,11 @@
         <v>289</v>
       </c>
       <c r="I70" s="13"/>
-      <c r="J70" s="8"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>261</v>
       </c>
@@ -4121,9 +4262,11 @@
         <v>289</v>
       </c>
       <c r="I71" s="13"/>
-      <c r="J71" s="16"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>253</v>
       </c>
@@ -4149,9 +4292,11 @@
         <v>289</v>
       </c>
       <c r="I72" s="13"/>
-      <c r="J72" s="16"/>
-    </row>
-    <row r="73" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>481</v>
       </c>
@@ -4177,9 +4322,11 @@
         <v>289</v>
       </c>
       <c r="I73" s="11"/>
-      <c r="J73" s="8"/>
-    </row>
-    <row r="74" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>168</v>
       </c>
@@ -4201,9 +4348,11 @@
         <v>289</v>
       </c>
       <c r="I74" s="11"/>
-      <c r="J74" s="8"/>
-    </row>
-    <row r="75" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>482</v>
       </c>
@@ -4225,9 +4374,11 @@
         <v>289</v>
       </c>
       <c r="I75" s="13"/>
-      <c r="J75" s="8"/>
-    </row>
-    <row r="76" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>169</v>
       </c>
@@ -4249,9 +4400,11 @@
         <v>289</v>
       </c>
       <c r="I76" s="13"/>
-      <c r="J76" s="8"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>170</v>
       </c>
@@ -4273,9 +4426,11 @@
         <v>289</v>
       </c>
       <c r="I77" s="11"/>
-      <c r="J77" s="16"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>254</v>
       </c>
@@ -4297,9 +4452,11 @@
         <v>289</v>
       </c>
       <c r="I78" s="13"/>
-      <c r="J78" s="16"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>171</v>
       </c>
@@ -4321,9 +4478,11 @@
         <v>289</v>
       </c>
       <c r="I79" s="13"/>
-      <c r="J79" s="16"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>172</v>
       </c>
@@ -4347,9 +4506,11 @@
         <v>289</v>
       </c>
       <c r="I80" s="13"/>
-      <c r="J80" s="16"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>173</v>
       </c>
@@ -4373,9 +4534,11 @@
         <v>289</v>
       </c>
       <c r="I81" s="7"/>
-      <c r="J81" s="16"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>483</v>
       </c>
@@ -4401,9 +4564,11 @@
         <v>289</v>
       </c>
       <c r="I82" s="7"/>
-      <c r="J82" s="16"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>174</v>
       </c>
@@ -4427,9 +4592,11 @@
         <v>289</v>
       </c>
       <c r="I83" s="13"/>
-      <c r="J83" s="16"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>484</v>
       </c>
@@ -4455,9 +4622,11 @@
         <v>151</v>
       </c>
       <c r="I84" s="13"/>
-      <c r="J84" s="16"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>285</v>
       </c>
@@ -4479,9 +4648,11 @@
         <v>289</v>
       </c>
       <c r="I85" s="13"/>
-      <c r="J85" s="16"/>
-    </row>
-    <row r="86" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>485</v>
       </c>
@@ -4507,9 +4678,11 @@
         <v>151</v>
       </c>
       <c r="I86" s="11"/>
-      <c r="J86" s="8"/>
-    </row>
-    <row r="87" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>486</v>
       </c>
@@ -4535,9 +4708,11 @@
         <v>289</v>
       </c>
       <c r="I87" s="13"/>
-      <c r="J87" s="8"/>
-    </row>
-    <row r="88" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>487</v>
       </c>
@@ -4563,9 +4738,11 @@
         <v>289</v>
       </c>
       <c r="I88" s="13"/>
-      <c r="J88" s="8"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>488</v>
       </c>
@@ -4591,9 +4768,11 @@
         <v>289</v>
       </c>
       <c r="I89" s="13"/>
-      <c r="J89" s="16"/>
-    </row>
-    <row r="90" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>175</v>
       </c>
@@ -4617,9 +4796,11 @@
         <v>289</v>
       </c>
       <c r="I90" s="13"/>
-      <c r="J90" s="8"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>489</v>
       </c>
@@ -4645,9 +4826,11 @@
         <v>289</v>
       </c>
       <c r="I91" s="13"/>
-      <c r="J91" s="16"/>
-    </row>
-    <row r="92" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>490</v>
       </c>
@@ -4673,9 +4856,11 @@
         <v>289</v>
       </c>
       <c r="I92" s="13"/>
-      <c r="J92" s="8"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>241</v>
       </c>
@@ -4699,9 +4884,11 @@
         <v>289</v>
       </c>
       <c r="I93" s="13"/>
-      <c r="J93" s="16"/>
-    </row>
-    <row r="94" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>491</v>
       </c>
@@ -4727,9 +4914,11 @@
         <v>289</v>
       </c>
       <c r="I94" s="13"/>
-      <c r="J94" s="8"/>
-    </row>
-    <row r="95" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>492</v>
       </c>
@@ -4755,9 +4944,11 @@
         <v>289</v>
       </c>
       <c r="I95" s="11"/>
-      <c r="J95" s="8"/>
-    </row>
-    <row r="96" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>493</v>
       </c>
@@ -4783,9 +4974,11 @@
         <v>289</v>
       </c>
       <c r="I96" s="7"/>
-      <c r="J96" s="8"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>494</v>
       </c>
@@ -4811,9 +5004,11 @@
         <v>289</v>
       </c>
       <c r="I97" s="13"/>
-      <c r="J97" s="16"/>
-    </row>
-    <row r="98" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>495</v>
       </c>
@@ -4839,9 +5034,11 @@
         <v>289</v>
       </c>
       <c r="I98" s="11"/>
-      <c r="J98" s="8"/>
-    </row>
-    <row r="99" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>496</v>
       </c>
@@ -4867,9 +5064,11 @@
         <v>289</v>
       </c>
       <c r="I99" s="11"/>
-      <c r="J99" s="8"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
         <v>286</v>
       </c>
@@ -4891,9 +5090,11 @@
         <v>289</v>
       </c>
       <c r="I100" s="11"/>
-      <c r="J100" s="16"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>176</v>
       </c>
@@ -4917,9 +5118,11 @@
         <v>289</v>
       </c>
       <c r="I101" s="7"/>
-      <c r="J101" s="16"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>242</v>
       </c>
@@ -4941,9 +5144,11 @@
         <v>289</v>
       </c>
       <c r="I102" s="13"/>
-      <c r="J102" s="16"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>240</v>
       </c>
@@ -4969,9 +5174,11 @@
         <v>289</v>
       </c>
       <c r="I103" s="7"/>
-      <c r="J103" s="16"/>
-    </row>
-    <row r="104" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>497</v>
       </c>
@@ -4997,9 +5204,11 @@
         <v>289</v>
       </c>
       <c r="I104" s="13"/>
-      <c r="J104" s="8"/>
-    </row>
-    <row r="105" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>177</v>
       </c>
@@ -5021,9 +5230,11 @@
         <v>289</v>
       </c>
       <c r="I105" s="11"/>
-      <c r="J105" s="8"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>178</v>
       </c>
@@ -5045,9 +5256,11 @@
         <v>289</v>
       </c>
       <c r="I106" s="7"/>
-      <c r="J106" s="16"/>
-    </row>
-    <row r="107" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>179</v>
       </c>
@@ -5069,9 +5282,11 @@
         <v>289</v>
       </c>
       <c r="I107" s="13"/>
-      <c r="J107" s="8"/>
-    </row>
-    <row r="108" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>498</v>
       </c>
@@ -5097,9 +5312,11 @@
         <v>289</v>
       </c>
       <c r="I108" s="11"/>
-      <c r="J108" s="8"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>499</v>
       </c>
@@ -5125,9 +5342,11 @@
         <v>289</v>
       </c>
       <c r="I109" s="11"/>
-      <c r="J109" s="16"/>
-    </row>
-    <row r="110" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>282</v>
       </c>
@@ -5149,9 +5368,11 @@
         <v>289</v>
       </c>
       <c r="I110" s="11"/>
-      <c r="J110" s="8"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>500</v>
       </c>
@@ -5177,9 +5398,11 @@
         <v>289</v>
       </c>
       <c r="I111" s="7"/>
-      <c r="J111" s="16"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>501</v>
       </c>
@@ -5205,9 +5428,11 @@
         <v>289</v>
       </c>
       <c r="I112" s="11"/>
-      <c r="J112" s="16"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>502</v>
       </c>
@@ -5229,9 +5454,11 @@
         <v>289</v>
       </c>
       <c r="I113" s="13"/>
-      <c r="J113" s="16"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>180</v>
       </c>
@@ -5253,9 +5480,11 @@
         <v>289</v>
       </c>
       <c r="I114" s="7"/>
-      <c r="J114" s="16"/>
-    </row>
-    <row r="115" spans="1:10" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>281</v>
       </c>
@@ -5277,9 +5506,11 @@
         <v>289</v>
       </c>
       <c r="I115" s="13"/>
-      <c r="J115" s="8"/>
-    </row>
-    <row r="116" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>503</v>
       </c>
@@ -5305,9 +5536,11 @@
         <v>151</v>
       </c>
       <c r="I116" s="7"/>
-      <c r="J116" s="8"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>504</v>
       </c>
@@ -5333,9 +5566,11 @@
         <v>289</v>
       </c>
       <c r="I117" s="13"/>
-      <c r="J117" s="16"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>181</v>
       </c>
@@ -5357,9 +5592,11 @@
         <v>289</v>
       </c>
       <c r="I118" s="13"/>
-      <c r="J118" s="16"/>
-    </row>
-    <row r="119" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>505</v>
       </c>
@@ -5385,9 +5622,11 @@
         <v>289</v>
       </c>
       <c r="I119" s="11"/>
-      <c r="J119" s="8"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>182</v>
       </c>
@@ -5411,9 +5650,11 @@
         <v>289</v>
       </c>
       <c r="I120" s="13"/>
-      <c r="J120" s="16"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>506</v>
       </c>
@@ -5439,9 +5680,11 @@
         <v>289</v>
       </c>
       <c r="I121" s="7"/>
-      <c r="J121" s="16"/>
-    </row>
-    <row r="122" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>507</v>
       </c>
@@ -5469,9 +5712,11 @@
       <c r="I122" s="13" t="s">
         <v>607</v>
       </c>
-      <c r="J122" s="8"/>
-    </row>
-    <row r="123" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>508</v>
       </c>
@@ -5499,9 +5744,11 @@
       <c r="I123" s="11" t="s">
         <v>608</v>
       </c>
-      <c r="J123" s="8"/>
-    </row>
-    <row r="124" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>509</v>
       </c>
@@ -5527,9 +5774,11 @@
         <v>289</v>
       </c>
       <c r="I124" s="13"/>
-      <c r="J124" s="8"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>510</v>
       </c>
@@ -5555,9 +5804,11 @@
         <v>289</v>
       </c>
       <c r="I125" s="13"/>
-      <c r="J125" s="16"/>
-    </row>
-    <row r="126" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>183</v>
       </c>
@@ -5579,9 +5830,11 @@
         <v>289</v>
       </c>
       <c r="I126" s="13"/>
-      <c r="J126" s="8"/>
-    </row>
-    <row r="127" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>184</v>
       </c>
@@ -5603,9 +5856,11 @@
         <v>289</v>
       </c>
       <c r="I127" s="11"/>
-      <c r="J127" s="8"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>185</v>
       </c>
@@ -5629,9 +5884,11 @@
         <v>289</v>
       </c>
       <c r="I128" s="13"/>
-      <c r="J128" s="16"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>255</v>
       </c>
@@ -5653,9 +5910,11 @@
         <v>289</v>
       </c>
       <c r="I129" s="13"/>
-      <c r="J129" s="16"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>511</v>
       </c>
@@ -5681,9 +5940,11 @@
         <v>289</v>
       </c>
       <c r="I130" s="13"/>
-      <c r="J130" s="16"/>
-    </row>
-    <row r="131" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>512</v>
       </c>
@@ -5709,9 +5970,11 @@
         <v>151</v>
       </c>
       <c r="I131" s="7"/>
-      <c r="J131" s="8"/>
-    </row>
-    <row r="132" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>280</v>
       </c>
@@ -5733,9 +5996,11 @@
         <v>289</v>
       </c>
       <c r="I132" s="11"/>
-      <c r="J132" s="8"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>513</v>
       </c>
@@ -5761,9 +6026,11 @@
         <v>289</v>
       </c>
       <c r="I133" s="13"/>
-      <c r="J133" s="16"/>
-    </row>
-    <row r="134" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>514</v>
       </c>
@@ -5789,9 +6056,11 @@
         <v>289</v>
       </c>
       <c r="I134" s="11"/>
-      <c r="J134" s="8"/>
-    </row>
-    <row r="135" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>515</v>
       </c>
@@ -5817,9 +6086,11 @@
         <v>289</v>
       </c>
       <c r="I135" s="7"/>
-      <c r="J135" s="8"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>516</v>
       </c>
@@ -5845,9 +6116,11 @@
         <v>289</v>
       </c>
       <c r="I136" s="7"/>
-      <c r="J136" s="16"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>243</v>
       </c>
@@ -5871,9 +6144,11 @@
         <v>289</v>
       </c>
       <c r="I137" s="7"/>
-      <c r="J137" s="16"/>
-    </row>
-    <row r="138" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>517</v>
       </c>
@@ -5899,9 +6174,11 @@
         <v>151</v>
       </c>
       <c r="I138" s="7"/>
-      <c r="J138" s="8"/>
-    </row>
-    <row r="139" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
         <v>186</v>
       </c>
@@ -5925,9 +6202,11 @@
         <v>289</v>
       </c>
       <c r="I139" s="11"/>
-      <c r="J139" s="8"/>
-    </row>
-    <row r="140" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>518</v>
       </c>
@@ -5953,9 +6232,11 @@
         <v>289</v>
       </c>
       <c r="I140" s="13"/>
-      <c r="J140" s="8"/>
-    </row>
-    <row r="141" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>187</v>
       </c>
@@ -5977,9 +6258,11 @@
         <v>289</v>
       </c>
       <c r="I141" s="7"/>
-      <c r="J141" s="8"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>188</v>
       </c>
@@ -6001,9 +6284,11 @@
         <v>289</v>
       </c>
       <c r="I142" s="7"/>
-      <c r="J142" s="16"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>519</v>
       </c>
@@ -6029,9 +6314,11 @@
         <v>289</v>
       </c>
       <c r="I143" s="13"/>
-      <c r="J143" s="16"/>
-    </row>
-    <row r="144" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>520</v>
       </c>
@@ -6057,9 +6344,11 @@
         <v>151</v>
       </c>
       <c r="I144" s="7"/>
-      <c r="J144" s="8"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>189</v>
       </c>
@@ -6083,9 +6372,11 @@
         <v>289</v>
       </c>
       <c r="I145" s="13"/>
-      <c r="J145" s="16"/>
-    </row>
-    <row r="146" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
         <v>521</v>
       </c>
@@ -6107,9 +6398,11 @@
         <v>289</v>
       </c>
       <c r="I146" s="14"/>
-      <c r="J146" s="8"/>
-    </row>
-    <row r="147" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>190</v>
       </c>
@@ -6131,9 +6424,11 @@
         <v>289</v>
       </c>
       <c r="I147" s="13"/>
-      <c r="J147" s="8"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>522</v>
       </c>
@@ -6159,9 +6454,11 @@
         <v>289</v>
       </c>
       <c r="I148" s="13"/>
-      <c r="J148" s="16"/>
-    </row>
-    <row r="149" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>191</v>
       </c>
@@ -6185,9 +6482,11 @@
         <v>289</v>
       </c>
       <c r="I149" s="13"/>
-      <c r="J149" s="8"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>192</v>
       </c>
@@ -6209,9 +6508,11 @@
         <v>289</v>
       </c>
       <c r="I150" s="7"/>
-      <c r="J150" s="16"/>
-    </row>
-    <row r="151" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>523</v>
       </c>
@@ -6237,9 +6538,11 @@
         <v>289</v>
       </c>
       <c r="I151" s="13"/>
-      <c r="J151" s="8"/>
-    </row>
-    <row r="152" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
         <v>524</v>
       </c>
@@ -6265,9 +6568,11 @@
         <v>151</v>
       </c>
       <c r="I152" s="13"/>
-      <c r="J152" s="8"/>
-    </row>
-    <row r="153" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
         <v>193</v>
       </c>
@@ -6291,9 +6596,11 @@
         <v>289</v>
       </c>
       <c r="I153" s="13"/>
-      <c r="J153" s="8"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>525</v>
       </c>
@@ -6319,9 +6626,11 @@
         <v>289</v>
       </c>
       <c r="I154" s="7"/>
-      <c r="J154" s="16"/>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>526</v>
       </c>
@@ -6347,9 +6656,11 @@
         <v>289</v>
       </c>
       <c r="I155" s="7"/>
-      <c r="J155" s="16"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>527</v>
       </c>
@@ -6375,9 +6686,11 @@
         <v>289</v>
       </c>
       <c r="I156" s="7"/>
-      <c r="J156" s="16"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>528</v>
       </c>
@@ -6403,9 +6716,11 @@
         <v>151</v>
       </c>
       <c r="I157" s="7"/>
-      <c r="J157" s="16"/>
-    </row>
-    <row r="158" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>529</v>
       </c>
@@ -6431,9 +6746,11 @@
         <v>289</v>
       </c>
       <c r="I158" s="13"/>
-      <c r="J158" s="8"/>
-    </row>
-    <row r="159" spans="1:10" s="2" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" s="2" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>194</v>
       </c>
@@ -6455,9 +6772,11 @@
         <v>289</v>
       </c>
       <c r="I159" s="13"/>
-      <c r="J159" s="8"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>256</v>
       </c>
@@ -6479,9 +6798,11 @@
         <v>289</v>
       </c>
       <c r="I160" s="13"/>
-      <c r="J160" s="16"/>
-    </row>
-    <row r="161" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
         <v>530</v>
       </c>
@@ -6507,9 +6828,11 @@
         <v>289</v>
       </c>
       <c r="I161" s="13"/>
-      <c r="J161" s="8"/>
-    </row>
-    <row r="162" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
         <v>279</v>
       </c>
@@ -6531,9 +6854,11 @@
         <v>289</v>
       </c>
       <c r="I162" s="13"/>
-      <c r="J162" s="8"/>
-    </row>
-    <row r="163" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
         <v>244</v>
       </c>
@@ -6557,9 +6882,11 @@
         <v>289</v>
       </c>
       <c r="I163" s="11"/>
-      <c r="J163" s="8"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>531</v>
       </c>
@@ -6585,9 +6912,11 @@
         <v>289</v>
       </c>
       <c r="I164" s="11"/>
-      <c r="J164" s="16"/>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="11" t="s">
         <v>532</v>
       </c>
@@ -6615,9 +6944,11 @@
       <c r="I165" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="J165" s="16"/>
-    </row>
-    <row r="166" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>533</v>
       </c>
@@ -6643,9 +6974,11 @@
         <v>289</v>
       </c>
       <c r="I166" s="11"/>
-      <c r="J166" s="8"/>
-    </row>
-    <row r="167" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>195</v>
       </c>
@@ -6669,9 +7002,11 @@
         <v>289</v>
       </c>
       <c r="I167" s="7"/>
-      <c r="J167" s="8"/>
-    </row>
-    <row r="168" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>534</v>
       </c>
@@ -6697,9 +7032,11 @@
         <v>289</v>
       </c>
       <c r="I168" s="13"/>
-      <c r="J168" s="8"/>
-    </row>
-    <row r="169" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>535</v>
       </c>
@@ -6725,9 +7062,11 @@
         <v>289</v>
       </c>
       <c r="I169" s="7"/>
-      <c r="J169" s="8"/>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
         <v>536</v>
       </c>
@@ -6753,9 +7092,11 @@
         <v>289</v>
       </c>
       <c r="I170" s="13"/>
-      <c r="J170" s="16"/>
-    </row>
-    <row r="171" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>537</v>
       </c>
@@ -6781,9 +7122,11 @@
         <v>289</v>
       </c>
       <c r="I171" s="7"/>
-      <c r="J171" s="8"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>538</v>
       </c>
@@ -6809,9 +7152,11 @@
         <v>151</v>
       </c>
       <c r="I172" s="13"/>
-      <c r="J172" s="16"/>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
         <v>196</v>
       </c>
@@ -6835,9 +7180,11 @@
         <v>289</v>
       </c>
       <c r="I173" s="13"/>
-      <c r="J173" s="16"/>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>539</v>
       </c>
@@ -6863,9 +7210,11 @@
         <v>289</v>
       </c>
       <c r="I174" s="7"/>
-      <c r="J174" s="16"/>
-    </row>
-    <row r="175" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
         <v>540</v>
       </c>
@@ -6891,9 +7240,11 @@
         <v>289</v>
       </c>
       <c r="I175" s="11"/>
-      <c r="J175" s="8"/>
-    </row>
-    <row r="176" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
         <v>541</v>
       </c>
@@ -6919,9 +7270,11 @@
         <v>289</v>
       </c>
       <c r="I176" s="13"/>
-      <c r="J176" s="8"/>
-    </row>
-    <row r="177" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
         <v>542</v>
       </c>
@@ -6947,9 +7300,11 @@
         <v>289</v>
       </c>
       <c r="I177" s="11"/>
-      <c r="J177" s="8"/>
-    </row>
-    <row r="178" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>197</v>
       </c>
@@ -6971,9 +7326,11 @@
         <v>289</v>
       </c>
       <c r="I178" s="7"/>
-      <c r="J178" s="8"/>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>198</v>
       </c>
@@ -6995,9 +7352,11 @@
         <v>289</v>
       </c>
       <c r="I179" s="7"/>
-      <c r="J179" s="16"/>
-    </row>
-    <row r="180" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J179" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
         <v>543</v>
       </c>
@@ -7023,9 +7382,11 @@
         <v>151</v>
       </c>
       <c r="I180" s="11"/>
-      <c r="J180" s="8"/>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>544</v>
       </c>
@@ -7051,9 +7412,11 @@
         <v>289</v>
       </c>
       <c r="I181" s="13"/>
-      <c r="J181" s="16"/>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J181" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="13" t="s">
         <v>545</v>
       </c>
@@ -7079,9 +7442,11 @@
         <v>289</v>
       </c>
       <c r="I182" s="13"/>
-      <c r="J182" s="16"/>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="13" t="s">
         <v>257</v>
       </c>
@@ -7103,9 +7468,11 @@
         <v>289</v>
       </c>
       <c r="I183" s="13"/>
-      <c r="J183" s="16"/>
-    </row>
-    <row r="184" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>546</v>
       </c>
@@ -7131,9 +7498,11 @@
         <v>289</v>
       </c>
       <c r="I184" s="7"/>
-      <c r="J184" s="8"/>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J184" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
         <v>245</v>
       </c>
@@ -7157,9 +7526,11 @@
         <v>289</v>
       </c>
       <c r="I185" s="13"/>
-      <c r="J185" s="16"/>
-    </row>
-    <row r="186" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="11" t="s">
         <v>199</v>
       </c>
@@ -7181,9 +7552,11 @@
         <v>289</v>
       </c>
       <c r="I186" s="11"/>
-      <c r="J186" s="8"/>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="13" t="s">
         <v>200</v>
       </c>
@@ -7207,9 +7580,11 @@
         <v>289</v>
       </c>
       <c r="I187" s="13"/>
-      <c r="J187" s="16"/>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
         <v>201</v>
       </c>
@@ -7231,9 +7606,11 @@
         <v>289</v>
       </c>
       <c r="I188" s="11"/>
-      <c r="J188" s="16"/>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J188" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>547</v>
       </c>
@@ -7259,9 +7636,11 @@
         <v>151</v>
       </c>
       <c r="I189" s="7"/>
-      <c r="J189" s="16"/>
-    </row>
-    <row r="190" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>548</v>
       </c>
@@ -7287,9 +7666,11 @@
         <v>151</v>
       </c>
       <c r="I190" s="7"/>
-      <c r="J190" s="8"/>
-    </row>
-    <row r="191" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="13" t="s">
         <v>549</v>
       </c>
@@ -7315,9 +7696,11 @@
         <v>151</v>
       </c>
       <c r="I191" s="13"/>
-      <c r="J191" s="8"/>
-    </row>
-    <row r="192" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="13" t="s">
         <v>550</v>
       </c>
@@ -7343,9 +7726,11 @@
         <v>289</v>
       </c>
       <c r="I192" s="13"/>
-      <c r="J192" s="8"/>
-    </row>
-    <row r="193" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>202</v>
       </c>
@@ -7369,9 +7754,11 @@
         <v>289</v>
       </c>
       <c r="I193" s="7"/>
-      <c r="J193" s="8"/>
-    </row>
-    <row r="194" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J193" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
         <v>203</v>
       </c>
@@ -7393,9 +7780,11 @@
         <v>289</v>
       </c>
       <c r="I194" s="13"/>
-      <c r="J194" s="8"/>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="13" t="s">
         <v>551</v>
       </c>
@@ -7421,9 +7810,11 @@
         <v>289</v>
       </c>
       <c r="I195" s="13"/>
-      <c r="J195" s="16"/>
-    </row>
-    <row r="196" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="13" t="s">
         <v>204</v>
       </c>
@@ -7445,9 +7836,11 @@
         <v>289</v>
       </c>
       <c r="I196" s="13"/>
-      <c r="J196" s="8"/>
-    </row>
-    <row r="197" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="13" t="s">
         <v>258</v>
       </c>
@@ -7471,9 +7864,11 @@
       <c r="I197" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="J197" s="8"/>
-    </row>
-    <row r="198" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="13" t="s">
         <v>552</v>
       </c>
@@ -7499,9 +7894,11 @@
         <v>289</v>
       </c>
       <c r="I198" s="13"/>
-      <c r="J198" s="8"/>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="13" t="s">
         <v>205</v>
       </c>
@@ -7523,9 +7920,11 @@
         <v>289</v>
       </c>
       <c r="I199" s="13"/>
-      <c r="J199" s="16"/>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="13" t="s">
         <v>206</v>
       </c>
@@ -7547,9 +7946,11 @@
         <v>289</v>
       </c>
       <c r="I200" s="13"/>
-      <c r="J200" s="16"/>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="18" t="s">
         <v>553</v>
       </c>
@@ -7575,9 +7976,11 @@
         <v>289</v>
       </c>
       <c r="I201" s="18"/>
-      <c r="J201" s="16"/>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J201" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="13" t="s">
         <v>554</v>
       </c>
@@ -7603,9 +8006,11 @@
         <v>289</v>
       </c>
       <c r="I202" s="13"/>
-      <c r="J202" s="16"/>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="11" t="s">
         <v>246</v>
       </c>
@@ -7627,9 +8032,11 @@
         <v>289</v>
       </c>
       <c r="I203" s="11"/>
-      <c r="J203" s="16"/>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>555</v>
       </c>
@@ -7655,9 +8062,11 @@
         <v>289</v>
       </c>
       <c r="I204" s="11"/>
-      <c r="J204" s="16"/>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="11" t="s">
         <v>556</v>
       </c>
@@ -7683,9 +8092,11 @@
         <v>289</v>
       </c>
       <c r="I205" s="11"/>
-      <c r="J205" s="16"/>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J205" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="11" t="s">
         <v>247</v>
       </c>
@@ -7709,9 +8120,11 @@
         <v>289</v>
       </c>
       <c r="I206" s="11"/>
-      <c r="J206" s="16"/>
-    </row>
-    <row r="207" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="11" t="s">
         <v>278</v>
       </c>
@@ -7733,9 +8146,11 @@
         <v>289</v>
       </c>
       <c r="I207" s="11"/>
-      <c r="J207" s="8"/>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
         <v>248</v>
       </c>
@@ -7759,9 +8174,11 @@
         <v>289</v>
       </c>
       <c r="I208" s="11"/>
-      <c r="J208" s="16"/>
-    </row>
-    <row r="209" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="11" t="s">
         <v>557</v>
       </c>
@@ -7787,9 +8204,11 @@
         <v>289</v>
       </c>
       <c r="I209" s="11"/>
-      <c r="J209" s="8"/>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="11" t="s">
         <v>263</v>
       </c>
@@ -7811,9 +8230,11 @@
         <v>289</v>
       </c>
       <c r="I210" s="11"/>
-      <c r="J210" s="16"/>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
         <v>207</v>
       </c>
@@ -7835,9 +8256,11 @@
         <v>289</v>
       </c>
       <c r="I211" s="7"/>
-      <c r="J211" s="16"/>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>558</v>
       </c>
@@ -7863,9 +8286,11 @@
         <v>289</v>
       </c>
       <c r="I212" s="7"/>
-      <c r="J212" s="16"/>
-    </row>
-    <row r="213" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J212" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>559</v>
       </c>
@@ -7891,9 +8316,11 @@
         <v>289</v>
       </c>
       <c r="I213" s="7"/>
-      <c r="J213" s="8"/>
-    </row>
-    <row r="214" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J213" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>208</v>
       </c>
@@ -7915,9 +8342,11 @@
         <v>289</v>
       </c>
       <c r="I214" s="7"/>
-      <c r="J214" s="8"/>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
         <v>277</v>
       </c>
@@ -7939,9 +8368,11 @@
         <v>289</v>
       </c>
       <c r="I215" s="12"/>
-      <c r="J215" s="16"/>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J215" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
         <v>276</v>
       </c>
@@ -7963,9 +8394,11 @@
         <v>289</v>
       </c>
       <c r="I216" s="12"/>
-      <c r="J216" s="16"/>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
         <v>560</v>
       </c>
@@ -7991,9 +8424,11 @@
         <v>289</v>
       </c>
       <c r="I217" s="12"/>
-      <c r="J217" s="16"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J217" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
         <v>561</v>
       </c>
@@ -8019,9 +8454,11 @@
         <v>289</v>
       </c>
       <c r="I218" s="12"/>
-      <c r="J218" s="16"/>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J218" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
         <v>275</v>
       </c>
@@ -8043,9 +8480,11 @@
         <v>289</v>
       </c>
       <c r="I219" s="12"/>
-      <c r="J219" s="16"/>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J219" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
         <v>209</v>
       </c>
@@ -8067,9 +8506,11 @@
         <v>289</v>
       </c>
       <c r="I220" s="12"/>
-      <c r="J220" s="16"/>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J220" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>210</v>
       </c>
@@ -8093,9 +8534,11 @@
         <v>289</v>
       </c>
       <c r="I221" s="12"/>
-      <c r="J221" s="16"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J221" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
         <v>562</v>
       </c>
@@ -8115,9 +8558,11 @@
         <v>151</v>
       </c>
       <c r="I222" s="12"/>
-      <c r="J222" s="16"/>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J222" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>563</v>
       </c>
@@ -8143,9 +8588,11 @@
         <v>151</v>
       </c>
       <c r="I223" s="12"/>
-      <c r="J223" s="16"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J223" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
         <v>274</v>
       </c>
@@ -8167,9 +8614,11 @@
         <v>289</v>
       </c>
       <c r="I224" s="12"/>
-      <c r="J224" s="16"/>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J224" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>249</v>
       </c>
@@ -8193,9 +8642,11 @@
         <v>289</v>
       </c>
       <c r="I225" s="12"/>
-      <c r="J225" s="16"/>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J225" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
         <v>564</v>
       </c>
@@ -8221,9 +8672,11 @@
         <v>289</v>
       </c>
       <c r="I226" s="12"/>
-      <c r="J226" s="16"/>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J226" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
         <v>565</v>
       </c>
@@ -8249,9 +8702,11 @@
         <v>289</v>
       </c>
       <c r="I227" s="12"/>
-      <c r="J227" s="16"/>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J227" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
         <v>566</v>
       </c>
@@ -8277,9 +8732,11 @@
         <v>289</v>
       </c>
       <c r="I228" s="12"/>
-      <c r="J228" s="16"/>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J228" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
         <v>211</v>
       </c>
@@ -8301,9 +8758,11 @@
         <v>289</v>
       </c>
       <c r="I229" s="12"/>
-      <c r="J229" s="16"/>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J229" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
         <v>212</v>
       </c>
@@ -8327,9 +8786,11 @@
         <v>289</v>
       </c>
       <c r="I230" s="12"/>
-      <c r="J230" s="16"/>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J230" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
         <v>213</v>
       </c>
@@ -8353,9 +8814,11 @@
         <v>289</v>
       </c>
       <c r="I231" s="12"/>
-      <c r="J231" s="16"/>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J231" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
         <v>567</v>
       </c>
@@ -8381,9 +8844,11 @@
         <v>289</v>
       </c>
       <c r="I232" s="12"/>
-      <c r="J232" s="16"/>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J232" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
         <v>214</v>
       </c>
@@ -8407,9 +8872,11 @@
         <v>289</v>
       </c>
       <c r="I233" s="12"/>
-      <c r="J233" s="16"/>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J233" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="12" t="s">
         <v>215</v>
       </c>
@@ -8433,9 +8900,11 @@
         <v>289</v>
       </c>
       <c r="I234" s="12"/>
-      <c r="J234" s="16"/>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J234" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
         <v>216</v>
       </c>
@@ -8459,9 +8928,11 @@
         <v>289</v>
       </c>
       <c r="I235" s="12"/>
-      <c r="J235" s="16"/>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J235" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="12" t="s">
         <v>568</v>
       </c>
@@ -8487,9 +8958,11 @@
         <v>289</v>
       </c>
       <c r="I236" s="12"/>
-      <c r="J236" s="16"/>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J236" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
         <v>569</v>
       </c>
@@ -8515,9 +8988,11 @@
         <v>289</v>
       </c>
       <c r="I237" s="12"/>
-      <c r="J237" s="16"/>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J237" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="12" t="s">
         <v>570</v>
       </c>
@@ -8543,9 +9018,11 @@
         <v>289</v>
       </c>
       <c r="I238" s="12"/>
-      <c r="J238" s="16"/>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J238" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
         <v>571</v>
       </c>
@@ -8571,9 +9048,11 @@
         <v>151</v>
       </c>
       <c r="I239" s="12"/>
-      <c r="J239" s="16"/>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J239" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="12" t="s">
         <v>572</v>
       </c>
@@ -8599,9 +9078,11 @@
         <v>289</v>
       </c>
       <c r="I240" s="12"/>
-      <c r="J240" s="16"/>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J240" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
         <v>573</v>
       </c>
@@ -8627,9 +9108,11 @@
         <v>289</v>
       </c>
       <c r="I241" s="12"/>
-      <c r="J241" s="16"/>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J241" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="12" t="s">
         <v>574</v>
       </c>
@@ -8655,9 +9138,11 @@
         <v>289</v>
       </c>
       <c r="I242" s="12"/>
-      <c r="J242" s="16"/>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J242" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
         <v>575</v>
       </c>
@@ -8683,9 +9168,11 @@
         <v>289</v>
       </c>
       <c r="I243" s="12"/>
-      <c r="J243" s="16"/>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J243" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
         <v>217</v>
       </c>
@@ -8709,9 +9196,11 @@
         <v>289</v>
       </c>
       <c r="I244" s="12"/>
-      <c r="J244" s="16"/>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J244" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
         <v>218</v>
       </c>
@@ -8735,9 +9224,11 @@
         <v>289</v>
       </c>
       <c r="I245" s="12"/>
-      <c r="J245" s="16"/>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J245" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
         <v>576</v>
       </c>
@@ -8763,9 +9254,11 @@
         <v>289</v>
       </c>
       <c r="I246" s="12"/>
-      <c r="J246" s="16"/>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J246" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>219</v>
       </c>
@@ -8789,9 +9282,11 @@
         <v>289</v>
       </c>
       <c r="I247" s="12"/>
-      <c r="J247" s="16"/>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J247" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
         <v>220</v>
       </c>
@@ -8815,9 +9310,11 @@
         <v>289</v>
       </c>
       <c r="I248" s="12"/>
-      <c r="J248" s="16"/>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J248" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
         <v>221</v>
       </c>
@@ -8841,9 +9338,11 @@
         <v>289</v>
       </c>
       <c r="I249" s="12"/>
-      <c r="J249" s="16"/>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J249" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
         <v>222</v>
       </c>
@@ -8865,9 +9364,11 @@
         <v>289</v>
       </c>
       <c r="I250" s="12"/>
-      <c r="J250" s="16"/>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J250" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
         <v>223</v>
       </c>
@@ -8891,9 +9392,11 @@
         <v>289</v>
       </c>
       <c r="I251" s="12"/>
-      <c r="J251" s="16"/>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J251" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
         <v>224</v>
       </c>
@@ -8917,9 +9420,11 @@
         <v>289</v>
       </c>
       <c r="I252" s="12"/>
-      <c r="J252" s="16"/>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J252" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
         <v>577</v>
       </c>
@@ -8945,9 +9450,11 @@
         <v>289</v>
       </c>
       <c r="I253" s="12"/>
-      <c r="J253" s="16"/>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J253" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
         <v>225</v>
       </c>
@@ -8971,9 +9478,11 @@
         <v>289</v>
       </c>
       <c r="I254" s="12"/>
-      <c r="J254" s="16"/>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J254" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
         <v>578</v>
       </c>
@@ -8995,9 +9504,11 @@
         <v>289</v>
       </c>
       <c r="I255" s="12"/>
-      <c r="J255" s="16"/>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J255" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
         <v>579</v>
       </c>
@@ -9023,9 +9534,11 @@
         <v>289</v>
       </c>
       <c r="I256" s="12"/>
-      <c r="J256" s="16"/>
-    </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J256" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
         <v>273</v>
       </c>
@@ -9047,9 +9560,11 @@
         <v>289</v>
       </c>
       <c r="I257" s="12"/>
-      <c r="J257" s="16"/>
-    </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J257" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
         <v>226</v>
       </c>
@@ -9071,9 +9586,11 @@
         <v>289</v>
       </c>
       <c r="I258" s="12"/>
-      <c r="J258" s="16"/>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J258" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
         <v>227</v>
       </c>
@@ -9095,9 +9612,11 @@
         <v>289</v>
       </c>
       <c r="I259" s="12"/>
-      <c r="J259" s="16"/>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J259" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="12" t="s">
         <v>228</v>
       </c>
@@ -9119,9 +9638,11 @@
         <v>289</v>
       </c>
       <c r="I260" s="12"/>
-      <c r="J260" s="16"/>
-    </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J260" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
         <v>272</v>
       </c>
@@ -9143,9 +9664,11 @@
         <v>289</v>
       </c>
       <c r="I261" s="12"/>
-      <c r="J261" s="16"/>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J261" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
         <v>580</v>
       </c>
@@ -9167,9 +9690,11 @@
         <v>289</v>
       </c>
       <c r="I262" s="12"/>
-      <c r="J262" s="16"/>
-    </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J262" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="12" t="s">
         <v>229</v>
       </c>
@@ -9191,9 +9716,11 @@
         <v>289</v>
       </c>
       <c r="I263" s="12"/>
-      <c r="J263" s="16"/>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J263" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
         <v>581</v>
       </c>
@@ -9219,9 +9746,11 @@
         <v>289</v>
       </c>
       <c r="I264" s="12"/>
-      <c r="J264" s="16"/>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J264" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
         <v>269</v>
       </c>
@@ -9243,9 +9772,11 @@
         <v>289</v>
       </c>
       <c r="I265" s="12"/>
-      <c r="J265" s="16"/>
-    </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J265" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="12" t="s">
         <v>582</v>
       </c>
@@ -9271,9 +9802,11 @@
         <v>289</v>
       </c>
       <c r="I266" s="12"/>
-      <c r="J266" s="16"/>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J266" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="12" t="s">
         <v>230</v>
       </c>
@@ -9295,9 +9828,11 @@
         <v>289</v>
       </c>
       <c r="I267" s="12"/>
-      <c r="J267" s="16"/>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J267" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="12" t="s">
         <v>583</v>
       </c>
@@ -9323,9 +9858,11 @@
         <v>289</v>
       </c>
       <c r="I268" s="12"/>
-      <c r="J268" s="16"/>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J268" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="12" t="s">
         <v>584</v>
       </c>
@@ -9351,9 +9888,11 @@
         <v>289</v>
       </c>
       <c r="I269" s="12"/>
-      <c r="J269" s="16"/>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J269" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
         <v>585</v>
       </c>
@@ -9379,9 +9918,11 @@
         <v>289</v>
       </c>
       <c r="I270" s="12"/>
-      <c r="J270" s="16"/>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J270" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
         <v>586</v>
       </c>
@@ -9407,9 +9948,11 @@
         <v>289</v>
       </c>
       <c r="I271" s="12"/>
-      <c r="J271" s="16"/>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J271" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="12" t="s">
         <v>271</v>
       </c>
@@ -9431,9 +9974,11 @@
         <v>289</v>
       </c>
       <c r="I272" s="12"/>
-      <c r="J272" s="16"/>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J272" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
         <v>268</v>
       </c>
@@ -9457,9 +10002,11 @@
       <c r="I273" s="12" t="s">
         <v>609</v>
       </c>
-      <c r="J273" s="16"/>
-    </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J273" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
         <v>587</v>
       </c>
@@ -9485,9 +10032,11 @@
         <v>289</v>
       </c>
       <c r="I274" s="12"/>
-      <c r="J274" s="16"/>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J274" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
         <v>231</v>
       </c>
@@ -9511,9 +10060,11 @@
         <v>289</v>
       </c>
       <c r="I275" s="12"/>
-      <c r="J275" s="16"/>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J275" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
         <v>588</v>
       </c>
@@ -9539,9 +10090,11 @@
         <v>289</v>
       </c>
       <c r="I276" s="12"/>
-      <c r="J276" s="16"/>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J276" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
         <v>232</v>
       </c>
@@ -9565,9 +10118,11 @@
         <v>289</v>
       </c>
       <c r="I277" s="12"/>
-      <c r="J277" s="16"/>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J277" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="12" t="s">
         <v>267</v>
       </c>
@@ -9589,9 +10144,11 @@
         <v>289</v>
       </c>
       <c r="I278" s="12"/>
-      <c r="J278" s="16"/>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J278" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
         <v>233</v>
       </c>
@@ -9615,9 +10172,11 @@
         <v>289</v>
       </c>
       <c r="I279" s="12"/>
-      <c r="J279" s="16"/>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J279" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="12" t="s">
         <v>250</v>
       </c>
@@ -9641,9 +10200,11 @@
         <v>289</v>
       </c>
       <c r="I280" s="12"/>
-      <c r="J280" s="16"/>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J280" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
         <v>234</v>
       </c>
@@ -9667,9 +10228,11 @@
         <v>289</v>
       </c>
       <c r="I281" s="12"/>
-      <c r="J281" s="16"/>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J281" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="12" t="s">
         <v>235</v>
       </c>
@@ -9693,9 +10256,11 @@
         <v>289</v>
       </c>
       <c r="I282" s="12"/>
-      <c r="J282" s="16"/>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J282" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
         <v>236</v>
       </c>
@@ -9719,9 +10284,11 @@
         <v>289</v>
       </c>
       <c r="I283" s="12"/>
-      <c r="J283" s="16"/>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J283" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="12" t="s">
         <v>251</v>
       </c>
@@ -9743,9 +10310,11 @@
         <v>289</v>
       </c>
       <c r="I284" s="12"/>
-      <c r="J284" s="16"/>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J284" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
         <v>589</v>
       </c>
@@ -9771,9 +10340,11 @@
         <v>289</v>
       </c>
       <c r="I285" s="12"/>
-      <c r="J285" s="16"/>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J285" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="12" t="s">
         <v>252</v>
       </c>
@@ -9795,9 +10366,11 @@
         <v>289</v>
       </c>
       <c r="I286" s="12"/>
-      <c r="J286" s="16"/>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J286" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
         <v>590</v>
       </c>
@@ -9823,9 +10396,11 @@
         <v>289</v>
       </c>
       <c r="I287" s="12"/>
-      <c r="J287" s="16"/>
-    </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J287" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="12" t="s">
         <v>591</v>
       </c>
@@ -9851,9 +10426,11 @@
         <v>289</v>
       </c>
       <c r="I288" s="12"/>
-      <c r="J288" s="16"/>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J288" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
         <v>592</v>
       </c>
@@ -9879,9 +10456,11 @@
         <v>289</v>
       </c>
       <c r="I289" s="12"/>
-      <c r="J289" s="16"/>
-    </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J289" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
         <v>259</v>
       </c>
@@ -9903,9 +10482,11 @@
         <v>289</v>
       </c>
       <c r="I290" s="12"/>
-      <c r="J290" s="16"/>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J290" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
         <v>593</v>
       </c>
@@ -9931,9 +10512,11 @@
         <v>289</v>
       </c>
       <c r="I291" s="12"/>
-      <c r="J291" s="16"/>
-    </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J291" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
         <v>237</v>
       </c>
@@ -9957,9 +10540,11 @@
       <c r="I292" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="J292" s="16"/>
-    </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J292" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
         <v>238</v>
       </c>
@@ -9983,9 +10568,11 @@
       <c r="I293" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J293" s="16"/>
-    </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J293" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
         <v>270</v>
       </c>
@@ -10007,9 +10594,11 @@
         <v>289</v>
       </c>
       <c r="I294" s="12"/>
-      <c r="J294" s="16"/>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J294" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
         <v>594</v>
       </c>
@@ -10035,9 +10624,11 @@
         <v>289</v>
       </c>
       <c r="I295" s="12"/>
-      <c r="J295" s="16"/>
-    </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J295" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="12" t="s">
         <v>266</v>
       </c>
@@ -10059,9 +10650,11 @@
         <v>289</v>
       </c>
       <c r="I296" s="12"/>
-      <c r="J296" s="16"/>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J296" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
         <v>288</v>
       </c>
@@ -10081,9 +10674,11 @@
         <v>289</v>
       </c>
       <c r="I297" s="12"/>
-      <c r="J297" s="16"/>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J297" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="12"/>
       <c r="B298" s="12"/>
       <c r="C298" s="12"/>
@@ -10095,7 +10690,7 @@
       <c r="I298" s="19"/>
       <c r="J298" s="16"/>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="6"/>
       <c r="C299" s="6"/>
       <c r="D299" s="6"/>

</xml_diff>